<commit_message>
worksheet serialization read_drawings. Transient commit.
</commit_message>
<xml_diff>
--- a/samples/data/image.xlsx
+++ b/samples/data/image.xlsx
@@ -111,6 +111,158 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="409575"/>
+          <a:ext cx="714375" cy="1514475"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Oval 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="314325" y="1333500"/>
+          <a:ext cx="695325" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="5-Point Star 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="2600325"/>
+          <a:ext cx="904875" cy="942975"/>
+        </a:xfrm>
+        <a:prstGeom prst="star5">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>

</xml_diff>